<commit_message>
backend routing for homepage, product page, user registration
</commit_message>
<xml_diff>
--- a/flask_project/data/awae_accounts.xlsx
+++ b/flask_project/data/awae_accounts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HDD documents\University\comp3900\capstone-project-3900-h10a-awae\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HDD documents\University\comp3900\capstone-project-3900-h10a-awae\flask_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7495785-5298-4CE3-B737-014070365B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B64F0C7-BE1F-424D-BD17-6CDE8C0F972B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,36 +31,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
   <si>
     <t>password</t>
-  </si>
-  <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>dob</t>
-  </si>
-  <si>
-    <t>joe</t>
-  </si>
-  <si>
-    <t>roberts</t>
-  </si>
-  <si>
-    <t>sarah</t>
-  </si>
-  <si>
-    <t>connor</t>
-  </si>
-  <si>
-    <t>john</t>
   </si>
   <si>
     <t>is_admin</t>
@@ -87,13 +63,7 @@
     <t>john@gmail.com</t>
   </si>
   <si>
-    <t>aaa</t>
-  </si>
-  <si>
-    <t>bbb</t>
-  </si>
-  <si>
-    <t>ccc</t>
+    <t>phone</t>
   </si>
 </sst>
 </file>
@@ -586,9 +556,8 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
   <cellStyles count="43">
@@ -946,21 +915,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
     <col min="2" max="2" width="18.21875" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
     <col min="7" max="7" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -968,87 +938,63 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>12345678</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>19841984</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>77776666</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <v>1984</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
       <c r="B4">
-        <v>1991</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
+        <v>19911991</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4">
+      <c r="D4">
+        <v>44447777</v>
+      </c>
+      <c r="E4">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added support for guest accounts
</commit_message>
<xml_diff>
--- a/flask_project/data/awae_accounts.xlsx
+++ b/flask_project/data/awae_accounts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HDD documents\University\comp3900\capstone-project-3900-h10a-awae\flask_project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acidi\Coding\capstone-project-3900-h10a-awae\flask_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B64F0C7-BE1F-424D-BD17-6CDE8C0F972B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8268E260-EC62-4A7D-838E-8DF41D90382D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="awae_accounts" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>phone</t>
+  </si>
+  <si>
+    <t>is_authenticated</t>
   </si>
 </sst>
 </file>
@@ -915,22 +918,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="14.21875" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -946,8 +949,11 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -963,8 +969,11 @@
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -980,8 +989,11 @@
       <c r="E3">
         <v>0</v>
       </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -996,6 +1008,9 @@
       </c>
       <c r="E4">
         <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>